<commit_message>
Update queries and data
</commit_message>
<xml_diff>
--- a/CHILD exemplar sources.xlsx
+++ b/CHILD exemplar sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25103"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ed4565/Development/polifonia/child-dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DD2B2D-36FE-054D-A7E6-D20E5291FC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3A02F84-A502-4FF9-8BA2-F84A686E1BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{039DAEF1-243F-44C7-9080-1A93E0D46CC0}"/>
   </bookViews>
@@ -34,11 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="134">
   <si>
     <t>Link</t>
   </si>
   <si>
+    <t>File</t>
+  </si>
+  <si>
     <t>Title</t>
   </si>
   <si>
@@ -57,43 +60,70 @@
     <t>A Memoir of Baron Bunsen, Late Minister Plenipotentiary and Envoy Extraordinary of His Majesty Frederic William IV. at the Court of St. James - Google Play</t>
   </si>
   <si>
+    <t>https://archive.org/download/dli.ministry.16991/E14072_Memoirs_of_Baron_Bunsen_vol_I_djvu.txt</t>
+  </si>
+  <si>
+    <t>LED entries refer to Google Books - text file downloaded from Internet Archive. Note: there are two volumes Vol 2 in Row 4.</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1433763797230</t>
+  </si>
+  <si>
+    <t>https://archive.org/download/dli.ministry.16991/E14073_Memoirs_of_Baron_Bunsen_vol_II_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1433948029619</t>
   </si>
   <si>
     <t>An Irish beauty of the regency; : Calvert, Frances Pery, Hon. Mrs., 1767-1859 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/cu31924028002743/cu31924028002743_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1530175082343</t>
   </si>
   <si>
     <t>Autobiography And Correspondence Of Mary Granville Vol 1 : Delany : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/autobiographyand002432mbp/autobiographyand002432mbp_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1434637762881</t>
   </si>
   <si>
     <t>BBC WW2 People's War | Listening Experience Database project (open.ac.uk)</t>
   </si>
   <si>
+    <t>No text file available</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1402131399589</t>
   </si>
   <si>
     <t>Delius, a life in letters : Delius, Frederick, 1862-1934 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://led.kmi.open.ac.uk/entity/lexp/1462050137013 </t>
+    <t xml:space="preserve">Not freely downloadable </t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1462050137013</t>
   </si>
   <si>
     <t>Friends and memories : White, Maude Valerie : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/friendsmemories00whituoft/friendsmemories00whituoft_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1449242879363</t>
   </si>
   <si>
     <t>http://www.southbankcentre.co.uk/about-us/history-and-archive/southbank-centre-archive</t>
   </si>
   <si>
-    <t>Southbank Centre Archive</t>
+    <t>Southbank Centre Archive - not a text file</t>
   </si>
   <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1401810883944</t>
@@ -102,90 +132,138 @@
     <t>https://books.google.co.uk/books/about/Letters_Written_During_a_Journey_to_Swit.html?id=uUMUAAAAQAAJ&amp;redir_esc=y</t>
   </si>
   <si>
+    <t>Letters Written During a Journey to Switzerland - no text file available</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1378126645</t>
   </si>
   <si>
     <t>Life and letters of Sir Charles Hallé; being an autobiography (1819-1860) with correspondence and diaries; edited by his son, C.E. Hallé, and his daughter, Marie Hallé : Hallé, Charles, (Sir) 1819-1895 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/lifelettersofsir00halluoft/lifelettersofsir00halluoft_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1426844423738</t>
   </si>
   <si>
     <t>Memoirs, journal, and correspondence of Thomas Moore : Moore, Thomas, 1779-1852 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/memoirsjournala19moorgoog/memoirsjournala19moorgoog_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1558351681445</t>
   </si>
   <si>
     <t>Memorials of Frederick Arthur Gore Ouseley, baronet, M.A., doctor and professor of music in the University of Oxford; precentor and canon residentiary in the cathedral church of Hereford: founder of St. Michael's, Tenbury, and first incumbent of that church : Havergal, Francis T. 1829-1890 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/cu31924022435766/cu31924022435766_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1436610229204</t>
   </si>
   <si>
     <t>Memories of a musician; reminiscences of seventy years of musical life : Ganz, Wilhelm, 1833-1914 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
-    <t xml:space="preserve">https://led.kmi.open.ac.uk/entity/lexp/1435839378719 </t>
+    <t>https://archive.org/download/memoriesofmusici00ganzuoft/memoriesofmusici00ganzuoft_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1435839378719</t>
   </si>
   <si>
     <t>Music And Manners : W. Beatty-Kingston : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://led.kmi.open.ac.uk/entity/lexp/1444079072687 </t>
+    <t>https://archive.org/download/musicandmanners005622mbp/musicandmanners005622mbp_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1444079072687</t>
   </si>
   <si>
     <t>MUSICAL MEMORIES : CAMILLE SAINT-SAENS : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/musicalmemories017451mbp/musicalmemories017451mbp_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1432295361459</t>
   </si>
   <si>
     <t>My musical life : Haweis, H. R. (Hugh Reginald), 1839-1901 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
-    <t xml:space="preserve">https://led.kmi.open.ac.uk/entity/lexp/1437644129613 </t>
+    <t>https://archive.org/download/mymusicallife00haweuoft/mymusicallife00haweuoft_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1437644129613</t>
   </si>
   <si>
     <t>Recent music and musicians as described in the diaries and correspondence of Ignatz Moscheles : Moscheles, Charlotte (Embden) d. 1889 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/recentmusicmusic00moscuoft/recentmusicmusic00moscuoft_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1426851801016</t>
   </si>
   <si>
     <t>Recollections of an old musician : Ryan, Thomas, 1827-1903 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
-    <t xml:space="preserve">https://led.kmi.open.ac.uk/entity/lexp/1448997318962 </t>
+    <t>https://archive.org/download/recollectionsofo00ryanuoft/recollectionsofo00ryanuoft_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1448997318962</t>
   </si>
   <si>
     <t>Reminiscences of Michael Kelly, of the King's Theatre, and Theatre Royal Drury Lane, including a period of nearly half a century; with original anecdotes of many distinguished persons, political, literary, and musical : Kelly, Michael, 1762-1826 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/reminiscencesofm02kellrich/reminiscencesofm02kellrich_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1426676012967</t>
   </si>
   <si>
     <t>Selected Correspondence Of Fryderyk Chopin : Arthur Hedley : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/selectedcorrespo002644mbp/selectedcorrespo002644mbp_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1425902082920</t>
   </si>
   <si>
     <t>The letters of Horace Walpole, fourth earl of Orford : Walpole, Horace, 1717-1797 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/lettershoracewa05toyngoog/lettershoracewa05toyngoog_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1534783369154</t>
   </si>
   <si>
     <t>The Life and Letters of Frances Baroness Bunsen : Augustus John Cuthbert Hare : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/lifeandlettersf02haregoog/lifeandlettersf02haregoog_djvu.txt</t>
+  </si>
+  <si>
+    <t>Note: there are two volumes - Vol 2 in Row 24</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1373900953</t>
   </si>
   <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1393500626807</t>
   </si>
   <si>
+    <t>https://archive.org/download/aby9330.0002.001.umich.edu/aby9330.0002.001.umich.edu_djvu.txt</t>
+  </si>
+  <si>
     <t>The Whiting Society of Ringers - Burstow - Reminiscences of Horsham</t>
   </si>
   <si>
@@ -195,119 +273,176 @@
     <t>Thirty years of musical life in London, 1870-1900 : Klein, Hermann, 1856-1934 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/thirtyyearsofmus00klei/thirtyyearsofmus00klei_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1438159538620</t>
   </si>
   <si>
     <t>My life and the story of the gospel hymns and of sacred songs and solos : Sankey, Ira D. (Ira David), 1840-1908 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/mylifeandthestor00sankuoft/mylifeandthestor00sankuoft_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1432211247717</t>
   </si>
   <si>
     <t>Musical Reminiscences: Past and Present : William Spark : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/musicalreminisc01spargoog/musicalreminisc01spargoog_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1467812208270</t>
+  </si>
+  <si>
     <t>Praeterita : John Rustin : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/Praeterita/Praeterita_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1384358284140</t>
   </si>
   <si>
     <t>Travels in the two Sicilies : Swinburne, Henry, 1743-1803 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/travelsintwosici01swin/travelsintwosici01swin_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1509032372128</t>
+  </si>
+  <si>
     <t>Italy : Morgan, Lady (Sydney), 1783-1859 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/italymorgan02morgiala/italymorgan02morgiala_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1513868732524</t>
   </si>
   <si>
     <t>A classical tour through Italy and Sicily : Richard Colt Hoare : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/aclassicaltourt00hoargoog/aclassicaltourt00hoargoog_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1517329129609</t>
+  </si>
+  <si>
     <t>Letters on Italy : illustrated by engravings : Castellan, A. L. (Antoine Laurent), 1772-1838 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/lettersonitalyil00cast/lettersonitalyil00cast_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1517843174581</t>
+  </si>
+  <si>
     <t>Rhymes and Recollections of a Hand-loom Weaver : William Thom : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/rhymesandrecoll01thomgoog/rhymesandrecoll01thomgoog_djvu.txt</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1524243384393</t>
+  </si>
+  <si>
     <t>Letters of Anna Seward: Written Between the Years 1784 and 1807 - Anna Seward - Google Books</t>
   </si>
   <si>
+    <t>https://archive.org/download/lettersannasewa09consgoog/lettersannasewa09consgoog_djvu.txt</t>
+  </si>
+  <si>
+    <t>LED entries refer to Google Books, text file downloaded from Internet Archive</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1365518167</t>
+  </si>
+  <si>
     <t>Music and friends; or, Pleasant recollections of a dilettante : Gardiner, William, 1770-1853 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/musicandfriends00gardgoog/musicandfriends00gardgoog_djvu.txt</t>
+  </si>
+  <si>
+    <t>Can only find Volume 3 on Internet Archive</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1396292425643</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1433879464338</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1433366995118</t>
   </si>
   <si>
     <t>Louis Spohr’s Autobiography, by Louis Spohr--The Project Gutenberg eBook</t>
   </si>
   <si>
+    <t>https://archive.org/download/LouisSpohrsAutobiography/LouisSpohrsAutobiography_djvu.txt</t>
+  </si>
+  <si>
+    <t>LED entries refer to Project Gutenberg, text file downloaded from Internet Archive</t>
+  </si>
+  <si>
+    <t>https://led.kmi.open.ac.uk/entity/lexp/1409482741175</t>
+  </si>
+  <si>
     <t>The diary of an invalid being the journal of a tour in pursuit of health in Portugal, Italy, Switzerland, and France in the years 1817, 1818, and 1819 : Matthews, Henry, 1789-1828. n 83188715 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/b22022235_0002/b22022235_0002_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1518781849818</t>
   </si>
   <si>
     <t>Reminiscences of the opera. By Benjamin Lumley : Lumley, Benjamin, 1812-1875 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/cu31924022334563/cu31924022334563_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1438607512684</t>
   </si>
   <si>
     <t>Musical Letters from Abroad: Including Detailed Accounts of the Birmingham ... : Lowell Mason : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/musicallettersf00unkngoog/musicallettersf00unkngoog_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1448279941918</t>
   </si>
   <si>
     <t>Music study in Germany : Fay, Amy, 1844-1928 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/musicstudyingerm00faya/musicstudyingerm00faya_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1417365409899</t>
   </si>
   <si>
     <t>Musings and memories of a musician : Henschel, George, Sir, 1850-1934 : Free Download, Borrow, and Streaming : Internet Archive</t>
   </si>
   <si>
+    <t>https://archive.org/download/cu31924022171585/cu31924022171585_djvu.txt</t>
+  </si>
+  <si>
     <t>https://led.kmi.open.ac.uk/entity/lexp/1452196853462</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1433763797230</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1433879464338</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1409482741175</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1396292425643</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1524243384393</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1365518167</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1467812208270</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1509032372128</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1517329129609</t>
-  </si>
-  <si>
-    <t>https://led.kmi.open.ac.uk/entity/lexp/1517843174581</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +462,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -353,18 +502,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -680,510 +838,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65004063-BA3B-4E89-A313-CBA917B38B8F}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="46.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="52.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="49.5" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="15.5" style="2"/>
+    <col min="1" max="2" width="55.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="52.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="15.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="45">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2"/>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="90">
+      <c r="A12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45">
+      <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="105">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60">
+      <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="60">
+      <c r="A19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="90">
+      <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45">
+      <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45">
+      <c r="A23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45">
+      <c r="A24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2"/>
+      <c r="B25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45">
+      <c r="A27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45">
+      <c r="A28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="1" t="s">
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>78</v>
+      <c r="D30" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30">
+      <c r="A31" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="45">
+      <c r="A34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45">
+      <c r="A35" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30">
+      <c r="A36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="45">
+      <c r="A37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="75">
+      <c r="A39" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="45">
+      <c r="A40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="45">
+      <c r="A41" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30">
+      <c r="A42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="45">
+      <c r="A43" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:B61">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:C63">
     <sortCondition ref="A3"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" display="https://archive.org/details/lifelettersofsir00halluoft" xr:uid="{22BECF86-8A28-4BDB-B215-69E0554D6AE9}"/>
-    <hyperlink ref="A9" r:id="rId2" xr:uid="{2FA6299E-AF8B-40A0-8C64-10EDA8BEC069}"/>
-    <hyperlink ref="A16" r:id="rId3" display="https://archive.org/details/musicalmemories017451mbp" xr:uid="{D3CCAF76-DD91-44B5-8277-93FAB1945A26}"/>
-    <hyperlink ref="A24" r:id="rId4" display="https://www.whitingsociety.org.uk/old-ringing-books/burstow-reminiscences-horsham.html" xr:uid="{5E55AD9F-9E0F-46F9-8723-D64531231ED1}"/>
-    <hyperlink ref="A17" r:id="rId5" display="https://archive.org/details/mymusicallife00haweuoft" xr:uid="{C70B03E7-636C-4ACE-B1C8-C1C223CA8AB7}"/>
-    <hyperlink ref="A25" r:id="rId6" display="https://archive.org/details/thirtyyearsofmus00klei" xr:uid="{DB6C602A-FD18-4CCE-A883-8B4CED33F5C9}"/>
-    <hyperlink ref="A5" r:id="rId7" display="https://archive.org/details/autobiographyand002432mbp" xr:uid="{557D3B76-5F9B-44D6-BB58-A42E1EE4FD78}"/>
-    <hyperlink ref="A15" r:id="rId8" display="https://archive.org/details/musicandmanners005622mbp" xr:uid="{8531D020-27C7-4019-9935-544C67FDA78E}"/>
-    <hyperlink ref="A19" r:id="rId9" display="https://archive.org/details/recollectionsofo00ryanuoft" xr:uid="{8F0349EB-25F0-4A30-8578-4208C35F57C8}"/>
-    <hyperlink ref="A8" r:id="rId10" display="https://archive.org/details/friendsmemories00whituoft" xr:uid="{429635C0-0C93-4B93-BD15-CDA4CCA51401}"/>
-    <hyperlink ref="A7" r:id="rId11" display="https://archive.org/details/deliuslifeinlett0000deli" xr:uid="{0CBE6507-23BE-476F-915E-18B2C1C1A393}"/>
-    <hyperlink ref="A22" r:id="rId12" display="https://archive.org/details/lettershoracewa05toyngoog" xr:uid="{B7563D76-364B-4F6F-8EB9-EFBD3AE80A13}"/>
-    <hyperlink ref="A12" r:id="rId13" display="https://archive.org/details/memoirsjournala19moorgoog" xr:uid="{1FC40709-22A1-42D8-BFAA-BA6C23BD7EDD}"/>
-    <hyperlink ref="A4" r:id="rId14" display="https://archive.org/details/cu31924028002743" xr:uid="{9D68FC73-166D-447B-A69E-4537DC75F4D8}"/>
+    <hyperlink ref="A12" r:id="rId1" display="https://archive.org/details/lifelettersofsir00halluoft" xr:uid="{22BECF86-8A28-4BDB-B215-69E0554D6AE9}"/>
+    <hyperlink ref="A10" r:id="rId2" xr:uid="{2FA6299E-AF8B-40A0-8C64-10EDA8BEC069}"/>
+    <hyperlink ref="A17" r:id="rId3" display="https://archive.org/details/musicalmemories017451mbp" xr:uid="{D3CCAF76-DD91-44B5-8277-93FAB1945A26}"/>
+    <hyperlink ref="A26" r:id="rId4" display="https://www.whitingsociety.org.uk/old-ringing-books/burstow-reminiscences-horsham.html" xr:uid="{5E55AD9F-9E0F-46F9-8723-D64531231ED1}"/>
+    <hyperlink ref="A18" r:id="rId5" display="https://archive.org/details/mymusicallife00haweuoft" xr:uid="{C70B03E7-636C-4ACE-B1C8-C1C223CA8AB7}"/>
+    <hyperlink ref="A27" r:id="rId6" display="https://archive.org/details/thirtyyearsofmus00klei" xr:uid="{DB6C602A-FD18-4CCE-A883-8B4CED33F5C9}"/>
+    <hyperlink ref="A6" r:id="rId7" display="https://archive.org/details/autobiographyand002432mbp" xr:uid="{557D3B76-5F9B-44D6-BB58-A42E1EE4FD78}"/>
+    <hyperlink ref="A16" r:id="rId8" display="https://archive.org/details/musicandmanners005622mbp" xr:uid="{8531D020-27C7-4019-9935-544C67FDA78E}"/>
+    <hyperlink ref="A20" r:id="rId9" display="https://archive.org/details/recollectionsofo00ryanuoft" xr:uid="{8F0349EB-25F0-4A30-8578-4208C35F57C8}"/>
+    <hyperlink ref="A9" r:id="rId10" display="https://archive.org/details/friendsmemories00whituoft" xr:uid="{429635C0-0C93-4B93-BD15-CDA4CCA51401}"/>
+    <hyperlink ref="A8" r:id="rId11" display="https://archive.org/details/deliuslifeinlett0000deli" xr:uid="{0CBE6507-23BE-476F-915E-18B2C1C1A393}"/>
+    <hyperlink ref="A23" r:id="rId12" display="https://archive.org/details/lettershoracewa05toyngoog" xr:uid="{B7563D76-364B-4F6F-8EB9-EFBD3AE80A13}"/>
+    <hyperlink ref="A13" r:id="rId13" display="https://archive.org/details/memoirsjournala19moorgoog" xr:uid="{1FC40709-22A1-42D8-BFAA-BA6C23BD7EDD}"/>
+    <hyperlink ref="A5" r:id="rId14" display="https://archive.org/details/cu31924028002743" xr:uid="{9D68FC73-166D-447B-A69E-4537DC75F4D8}"/>
     <hyperlink ref="A3" r:id="rId15" display="https://play.google.com/books/reader?id=qhmpSZqCP-cC&amp;hl=en&amp;pg=GBS.PA76" xr:uid="{289F5B39-8DEF-4127-BBFA-793658DBB46A}"/>
-    <hyperlink ref="A20" r:id="rId16" display="https://archive.org/details/reminiscencesofm02kellrich" xr:uid="{20F03E2E-E5E9-45AD-AD2D-158FF5A88B8A}"/>
-    <hyperlink ref="A21" r:id="rId17" display="https://archive.org/details/selectedcorrespo002644mbp" xr:uid="{2F43C843-68A2-4C89-AC83-D273074D7B02}"/>
-    <hyperlink ref="A13" r:id="rId18" display="https://archive.org/details/cu31924022435766" xr:uid="{4A57A42A-A67B-4E6F-B789-F8512FCEECFE}"/>
-    <hyperlink ref="A18" r:id="rId19" display="https://archive.org/details/recentmusicmusic00moscuoft" xr:uid="{8F784AA7-329D-4DFF-8A1B-5AB313652BA1}"/>
-    <hyperlink ref="A10" r:id="rId20" xr:uid="{463200A7-0757-4B41-AF35-EB586FB29347}"/>
-    <hyperlink ref="A23" r:id="rId21" display="https://archive.org/details/lifeandlettersf02haregoog" xr:uid="{0960300D-B571-41A5-AC8F-D8F27FC5FC5A}"/>
-    <hyperlink ref="A14" r:id="rId22" display="https://archive.org/details/memoriesofmusici00ganzuoft" xr:uid="{E960BBCC-BE8D-48A3-A378-9F180C754939}"/>
-    <hyperlink ref="A26" r:id="rId23" display="https://archive.org/details/mylifeandthestor00sankuoft" xr:uid="{044DAD28-B1A1-43CC-AE5B-92EFD02D6FDC}"/>
-    <hyperlink ref="A6" r:id="rId24" display="https://led.kmi.open.ac.uk/browse/http%3A-_--_-data.open.ac.uk-_-led-_-source-_-BBC%2BWW2%2BPeople%27s%2BWar-_-1402130847379" xr:uid="{8E2ACE3F-6703-4E67-AD34-273B492D1F83}"/>
-    <hyperlink ref="A27" r:id="rId25" display="https://archive.org/details/musicalreminisc01spargoog" xr:uid="{E7185CF7-8EA9-4239-AEC6-B0DC054ABE6E}"/>
-    <hyperlink ref="A28" r:id="rId26" display="https://archive.org/details/Praeterita" xr:uid="{C90D93F5-9F0E-4455-946B-1E1013D59FCB}"/>
-    <hyperlink ref="A29" r:id="rId27" display="https://archive.org/details/travelsintwosici01swin" xr:uid="{574EA48C-F40A-4E62-9971-6716CDA1F8CE}"/>
-    <hyperlink ref="A30" r:id="rId28" display="https://archive.org/details/italymorgan02morgiala" xr:uid="{36A8334F-EA73-44C8-9F50-88E493E44D4B}"/>
-    <hyperlink ref="A31" r:id="rId29" display="https://archive.org/details/aclassicaltourt00hoargoog" xr:uid="{2EAF7A69-7660-4D67-A247-637D8B14D45F}"/>
-    <hyperlink ref="A32" r:id="rId30" display="https://archive.org/details/lettersonitalyil00cast" xr:uid="{B870724F-483A-4093-BB49-D6F336439FDC}"/>
-    <hyperlink ref="A33" r:id="rId31" display="https://archive.org/details/rhymesandrecoll01thomgoog" xr:uid="{419C99C6-C9ED-403C-88E4-350EF903739E}"/>
-    <hyperlink ref="A34" r:id="rId32" display="https://books.google.co.uk/books/about/Letters_of_Anna_Seward.html?id=CXs4AAAAIAAJ&amp;redir_esc=y" xr:uid="{A8794810-8C37-42A0-9CBC-49B61F2F8E8E}"/>
-    <hyperlink ref="A35" r:id="rId33" display="https://archive.org/details/musicandfriends00gardgoog" xr:uid="{AD249B90-D31E-4BC2-B57B-D86F93304DDD}"/>
-    <hyperlink ref="A36" r:id="rId34" display="https://www.gutenberg.org/files/45997/45997-h/45997-h.htm" xr:uid="{D6692868-7067-435C-B0DA-E2A693F97DE8}"/>
-    <hyperlink ref="A37" r:id="rId35" display="https://archive.org/details/b22022235_0002" xr:uid="{6EAD3734-2DAB-4703-A99A-46070C4958C2}"/>
-    <hyperlink ref="A38" r:id="rId36" display="https://archive.org/details/cu31924022334563" xr:uid="{BD201A1C-BD73-457C-8F1D-AFAE42F661C8}"/>
-    <hyperlink ref="A39" r:id="rId37" display="https://archive.org/details/musicallettersf00unkngoog" xr:uid="{D436B3BB-B792-4A12-A5FD-7C0D7131B079}"/>
-    <hyperlink ref="A40" r:id="rId38" display="https://archive.org/details/musicstudyingerm00faya" xr:uid="{F046EA5C-388F-4146-9CF1-DA576486F2C4}"/>
-    <hyperlink ref="A41" r:id="rId39" display="https://archive.org/details/cu31924022171585" xr:uid="{3EE43047-5D65-4E00-A900-EBFABF6AAFBF}"/>
-    <hyperlink ref="C4" r:id="rId40" xr:uid="{0074BB52-5D2E-42AC-9B1B-FB59B64733C5}"/>
-    <hyperlink ref="C6" r:id="rId41" xr:uid="{842BE7CC-BB21-40AB-959A-4FFE7C372A94}"/>
-    <hyperlink ref="C5" r:id="rId42" xr:uid="{2BCDD742-2428-4561-9156-30558FAFF2D2}"/>
-    <hyperlink ref="C8" r:id="rId43" xr:uid="{3922FD87-0E30-4E39-8999-3247B625AA2D}"/>
-    <hyperlink ref="C9" r:id="rId44" xr:uid="{70B08106-33E4-42A7-964F-254116063D81}"/>
-    <hyperlink ref="C11" r:id="rId45" xr:uid="{D37D1C01-0A81-4580-B382-A18197EB39DF}"/>
-    <hyperlink ref="C12" r:id="rId46" xr:uid="{25AA7084-DE37-490D-8E30-274640448294}"/>
-    <hyperlink ref="C13" r:id="rId47" xr:uid="{772BE2A6-7185-476A-8258-8E2BF0AC8910}"/>
-    <hyperlink ref="C14" r:id="rId48" xr:uid="{F5557B1D-CFF9-4193-BB65-71D2E2FAA85D}"/>
-    <hyperlink ref="C16" r:id="rId49" xr:uid="{83E9DB42-E239-44B3-9652-BD9F88605296}"/>
-    <hyperlink ref="C17" r:id="rId50" xr:uid="{5C667804-A9C7-4002-B82D-C1BDA288AE11}"/>
-    <hyperlink ref="C18" r:id="rId51" xr:uid="{204B7B76-2FAE-45B3-8740-A455B7D1EFB5}"/>
-    <hyperlink ref="C19" r:id="rId52" xr:uid="{3C73381C-D150-474F-8E5C-4228917EA277}"/>
-    <hyperlink ref="C20" r:id="rId53" xr:uid="{2A9B5A82-0880-433D-9396-88D02568F70A}"/>
-    <hyperlink ref="C21" r:id="rId54" xr:uid="{83F1BCB9-459E-42B0-BFCE-394ACD4FF14F}"/>
-    <hyperlink ref="C22" r:id="rId55" xr:uid="{9BCE4A25-6452-4655-A813-BDFC8AE0CB41}"/>
-    <hyperlink ref="C23" r:id="rId56" xr:uid="{2D8478A2-C2A6-4579-A5E4-04CB1615DA0F}"/>
-    <hyperlink ref="C24" r:id="rId57" xr:uid="{DEEF4465-AC43-4AEB-BB73-466A35D666A7}"/>
-    <hyperlink ref="C25" r:id="rId58" xr:uid="{7A8CBC73-B43D-44FA-B020-9A1D0FB840DE}"/>
-    <hyperlink ref="C26" r:id="rId59" xr:uid="{26CC39CC-08C5-41C7-9D7D-42C9B1168401}"/>
-    <hyperlink ref="C27" r:id="rId60" xr:uid="{FA53134B-E380-4810-B949-DD380CACF17D}"/>
-    <hyperlink ref="C28" r:id="rId61" xr:uid="{12E3B7BC-4C69-406B-A427-F4E6A3744E2E}"/>
-    <hyperlink ref="C29" r:id="rId62" xr:uid="{54460B4C-8FD5-423B-8CF7-0939EBF6BFE9}"/>
-    <hyperlink ref="C30" r:id="rId63" xr:uid="{89260570-A08B-46F2-87AB-A3A481EB09B3}"/>
-    <hyperlink ref="C31" r:id="rId64" xr:uid="{1DCAE6F2-85B6-4F9B-B7ED-AAEA48AB004D}"/>
-    <hyperlink ref="C32" r:id="rId65" xr:uid="{BC9A3590-BCCF-43F7-906E-CACFD1C33A9C}"/>
-    <hyperlink ref="C33" r:id="rId66" xr:uid="{E5D617CA-144D-42DB-A5DD-C04FAF6EB2D4}"/>
-    <hyperlink ref="C34" r:id="rId67" xr:uid="{BE67B56F-20C6-4B9C-A16B-7618730124C2}"/>
-    <hyperlink ref="C35" r:id="rId68" xr:uid="{17D9A1B4-F907-477C-B7F6-7CFC63295253}"/>
-    <hyperlink ref="D35" r:id="rId69" xr:uid="{01710E5D-5763-4745-BBE6-A348B327308A}"/>
-    <hyperlink ref="E35" r:id="rId70" xr:uid="{C1CC9E72-747E-4617-8FBF-70469A4739A1}"/>
-    <hyperlink ref="D23" r:id="rId71" xr:uid="{0FD98FA1-CC85-418A-9A6F-07665EA1181C}"/>
-    <hyperlink ref="C3" r:id="rId72" xr:uid="{EC112B3E-0C5E-4DAB-B8CA-7B5F0493EB7C}"/>
-    <hyperlink ref="D3" r:id="rId73" xr:uid="{1EF01DC3-0F04-4D19-8135-B0E4A63C4FD8}"/>
-    <hyperlink ref="C36" r:id="rId74" xr:uid="{9D0E0AB9-6B9E-41CA-9385-BAEE21F38743}"/>
-    <hyperlink ref="C37" r:id="rId75" xr:uid="{21EBD295-C635-4CB1-8DD9-F23693D5DE79}"/>
-    <hyperlink ref="C38" r:id="rId76" xr:uid="{AADA5EE0-021F-495A-ABC9-6DFFEE4535F4}"/>
-    <hyperlink ref="C39" r:id="rId77" xr:uid="{ED6D3DD6-F47C-423B-BA8E-469B1F30B23D}"/>
-    <hyperlink ref="C40" r:id="rId78" xr:uid="{84DA6015-0917-45BF-9D49-28AD5B77DB18}"/>
-    <hyperlink ref="C41" r:id="rId79" xr:uid="{B57B5D33-994F-427A-B63C-236E6DCE702E}"/>
-    <hyperlink ref="C10" r:id="rId80" xr:uid="{7A4F1120-331D-4CFE-90DB-A44959F74187}"/>
+    <hyperlink ref="A21" r:id="rId16" display="https://archive.org/details/reminiscencesofm02kellrich" xr:uid="{20F03E2E-E5E9-45AD-AD2D-158FF5A88B8A}"/>
+    <hyperlink ref="A22" r:id="rId17" display="https://archive.org/details/selectedcorrespo002644mbp" xr:uid="{2F43C843-68A2-4C89-AC83-D273074D7B02}"/>
+    <hyperlink ref="A14" r:id="rId18" display="https://archive.org/details/cu31924022435766" xr:uid="{4A57A42A-A67B-4E6F-B789-F8512FCEECFE}"/>
+    <hyperlink ref="A19" r:id="rId19" display="https://archive.org/details/recentmusicmusic00moscuoft" xr:uid="{8F784AA7-329D-4DFF-8A1B-5AB313652BA1}"/>
+    <hyperlink ref="A11" r:id="rId20" xr:uid="{463200A7-0757-4B41-AF35-EB586FB29347}"/>
+    <hyperlink ref="A24" r:id="rId21" display="https://archive.org/details/lifeandlettersf02haregoog" xr:uid="{0960300D-B571-41A5-AC8F-D8F27FC5FC5A}"/>
+    <hyperlink ref="A15" r:id="rId22" display="https://archive.org/details/memoriesofmusici00ganzuoft" xr:uid="{E960BBCC-BE8D-48A3-A378-9F180C754939}"/>
+    <hyperlink ref="A28" r:id="rId23" display="https://archive.org/details/mylifeandthestor00sankuoft" xr:uid="{044DAD28-B1A1-43CC-AE5B-92EFD02D6FDC}"/>
+    <hyperlink ref="A7" r:id="rId24" display="https://led.kmi.open.ac.uk/browse/http%3A-_--_-data.open.ac.uk-_-led-_-source-_-BBC%2BWW2%2BPeople%27s%2BWar-_-1402130847379" xr:uid="{8E2ACE3F-6703-4E67-AD34-273B492D1F83}"/>
+    <hyperlink ref="A29" r:id="rId25" display="https://archive.org/details/musicalreminisc01spargoog" xr:uid="{E7185CF7-8EA9-4239-AEC6-B0DC054ABE6E}"/>
+    <hyperlink ref="A30" r:id="rId26" display="https://archive.org/details/Praeterita" xr:uid="{C90D93F5-9F0E-4455-946B-1E1013D59FCB}"/>
+    <hyperlink ref="A31" r:id="rId27" display="https://archive.org/details/travelsintwosici01swin" xr:uid="{574EA48C-F40A-4E62-9971-6716CDA1F8CE}"/>
+    <hyperlink ref="A32" r:id="rId28" display="https://archive.org/details/italymorgan02morgiala" xr:uid="{36A8334F-EA73-44C8-9F50-88E493E44D4B}"/>
+    <hyperlink ref="A33" r:id="rId29" display="https://archive.org/details/aclassicaltourt00hoargoog" xr:uid="{2EAF7A69-7660-4D67-A247-637D8B14D45F}"/>
+    <hyperlink ref="A34" r:id="rId30" display="https://archive.org/details/lettersonitalyil00cast" xr:uid="{B870724F-483A-4093-BB49-D6F336439FDC}"/>
+    <hyperlink ref="A35" r:id="rId31" display="https://archive.org/details/rhymesandrecoll01thomgoog" xr:uid="{419C99C6-C9ED-403C-88E4-350EF903739E}"/>
+    <hyperlink ref="A36" r:id="rId32" display="https://books.google.co.uk/books/about/Letters_of_Anna_Seward.html?id=CXs4AAAAIAAJ&amp;redir_esc=y" xr:uid="{A8794810-8C37-42A0-9CBC-49B61F2F8E8E}"/>
+    <hyperlink ref="A37" r:id="rId33" display="https://archive.org/details/musicandfriends00gardgoog" xr:uid="{AD249B90-D31E-4BC2-B57B-D86F93304DDD}"/>
+    <hyperlink ref="A38" r:id="rId34" display="https://www.gutenberg.org/files/45997/45997-h/45997-h.htm" xr:uid="{D6692868-7067-435C-B0DA-E2A693F97DE8}"/>
+    <hyperlink ref="A39" r:id="rId35" display="https://archive.org/details/b22022235_0002" xr:uid="{6EAD3734-2DAB-4703-A99A-46070C4958C2}"/>
+    <hyperlink ref="A40" r:id="rId36" display="https://archive.org/details/cu31924022334563" xr:uid="{BD201A1C-BD73-457C-8F1D-AFAE42F661C8}"/>
+    <hyperlink ref="A41" r:id="rId37" display="https://archive.org/details/musicallettersf00unkngoog" xr:uid="{D436B3BB-B792-4A12-A5FD-7C0D7131B079}"/>
+    <hyperlink ref="A42" r:id="rId38" display="https://archive.org/details/musicstudyingerm00faya" xr:uid="{F046EA5C-388F-4146-9CF1-DA576486F2C4}"/>
+    <hyperlink ref="A43" r:id="rId39" display="https://archive.org/details/cu31924022171585" xr:uid="{3EE43047-5D65-4E00-A900-EBFABF6AAFBF}"/>
+    <hyperlink ref="D5" r:id="rId40" xr:uid="{0074BB52-5D2E-42AC-9B1B-FB59B64733C5}"/>
+    <hyperlink ref="D7" r:id="rId41" xr:uid="{842BE7CC-BB21-40AB-959A-4FFE7C372A94}"/>
+    <hyperlink ref="D6" r:id="rId42" xr:uid="{2BCDD742-2428-4561-9156-30558FAFF2D2}"/>
+    <hyperlink ref="D9" r:id="rId43" xr:uid="{3922FD87-0E30-4E39-8999-3247B625AA2D}"/>
+    <hyperlink ref="D10" r:id="rId44" xr:uid="{70B08106-33E4-42A7-964F-254116063D81}"/>
+    <hyperlink ref="D12" r:id="rId45" xr:uid="{D37D1C01-0A81-4580-B382-A18197EB39DF}"/>
+    <hyperlink ref="D13" r:id="rId46" xr:uid="{25AA7084-DE37-490D-8E30-274640448294}"/>
+    <hyperlink ref="D14" r:id="rId47" xr:uid="{772BE2A6-7185-476A-8258-8E2BF0AC8910}"/>
+    <hyperlink ref="D15" r:id="rId48" xr:uid="{F5557B1D-CFF9-4193-BB65-71D2E2FAA85D}"/>
+    <hyperlink ref="D17" r:id="rId49" xr:uid="{83E9DB42-E239-44B3-9652-BD9F88605296}"/>
+    <hyperlink ref="D18" r:id="rId50" xr:uid="{5C667804-A9C7-4002-B82D-C1BDA288AE11}"/>
+    <hyperlink ref="D19" r:id="rId51" xr:uid="{204B7B76-2FAE-45B3-8740-A455B7D1EFB5}"/>
+    <hyperlink ref="D20" r:id="rId52" xr:uid="{3C73381C-D150-474F-8E5C-4228917EA277}"/>
+    <hyperlink ref="D21" r:id="rId53" xr:uid="{2A9B5A82-0880-433D-9396-88D02568F70A}"/>
+    <hyperlink ref="D22" r:id="rId54" xr:uid="{83F1BCB9-459E-42B0-BFCE-394ACD4FF14F}"/>
+    <hyperlink ref="D23" r:id="rId55" xr:uid="{9BCE4A25-6452-4655-A813-BDFC8AE0CB41}"/>
+    <hyperlink ref="D24" r:id="rId56" xr:uid="{2D8478A2-C2A6-4579-A5E4-04CB1615DA0F}"/>
+    <hyperlink ref="D26" r:id="rId57" xr:uid="{DEEF4465-AC43-4AEB-BB73-466A35D666A7}"/>
+    <hyperlink ref="D27" r:id="rId58" xr:uid="{7A8CBC73-B43D-44FA-B020-9A1D0FB840DE}"/>
+    <hyperlink ref="D28" r:id="rId59" xr:uid="{26CC39CC-08C5-41C7-9D7D-42C9B1168401}"/>
+    <hyperlink ref="D29" r:id="rId60" xr:uid="{FA53134B-E380-4810-B949-DD380CACF17D}"/>
+    <hyperlink ref="D30" r:id="rId61" xr:uid="{12E3B7BC-4C69-406B-A427-F4E6A3744E2E}"/>
+    <hyperlink ref="D31" r:id="rId62" xr:uid="{54460B4C-8FD5-423B-8CF7-0939EBF6BFE9}"/>
+    <hyperlink ref="D32" r:id="rId63" xr:uid="{89260570-A08B-46F2-87AB-A3A481EB09B3}"/>
+    <hyperlink ref="D33" r:id="rId64" xr:uid="{1DCAE6F2-85B6-4F9B-B7ED-AAEA48AB004D}"/>
+    <hyperlink ref="D34" r:id="rId65" xr:uid="{BC9A3590-BCCF-43F7-906E-CACFD1C33A9C}"/>
+    <hyperlink ref="D35" r:id="rId66" xr:uid="{E5D617CA-144D-42DB-A5DD-C04FAF6EB2D4}"/>
+    <hyperlink ref="D36" r:id="rId67" xr:uid="{BE67B56F-20C6-4B9C-A16B-7618730124C2}"/>
+    <hyperlink ref="D37" r:id="rId68" xr:uid="{17D9A1B4-F907-477C-B7F6-7CFC63295253}"/>
+    <hyperlink ref="E37" r:id="rId69" xr:uid="{01710E5D-5763-4745-BBE6-A348B327308A}"/>
+    <hyperlink ref="F37" r:id="rId70" xr:uid="{C1CC9E72-747E-4617-8FBF-70469A4739A1}"/>
+    <hyperlink ref="E24" r:id="rId71" xr:uid="{0FD98FA1-CC85-418A-9A6F-07665EA1181C}"/>
+    <hyperlink ref="D3" r:id="rId72" xr:uid="{EC112B3E-0C5E-4DAB-B8CA-7B5F0493EB7C}"/>
+    <hyperlink ref="E4" r:id="rId73" xr:uid="{1EF01DC3-0F04-4D19-8135-B0E4A63C4FD8}"/>
+    <hyperlink ref="D38" r:id="rId74" xr:uid="{9D0E0AB9-6B9E-41CA-9385-BAEE21F38743}"/>
+    <hyperlink ref="D39" r:id="rId75" xr:uid="{21EBD295-C635-4CB1-8DD9-F23693D5DE79}"/>
+    <hyperlink ref="D40" r:id="rId76" xr:uid="{AADA5EE0-021F-495A-ABC9-6DFFEE4535F4}"/>
+    <hyperlink ref="D41" r:id="rId77" xr:uid="{ED6D3DD6-F47C-423B-BA8E-469B1F30B23D}"/>
+    <hyperlink ref="D42" r:id="rId78" xr:uid="{84DA6015-0917-45BF-9D49-28AD5B77DB18}"/>
+    <hyperlink ref="D43" r:id="rId79" xr:uid="{B57B5D33-994F-427A-B63C-236E6DCE702E}"/>
+    <hyperlink ref="D11" r:id="rId80" xr:uid="{7A4F1120-331D-4CFE-90DB-A44959F74187}"/>
+    <hyperlink ref="B9" r:id="rId81" xr:uid="{546DBCBA-81B1-4686-8207-85005A6A2827}"/>
+    <hyperlink ref="B5" r:id="rId82" xr:uid="{BB5F64D5-4F0A-4DFE-B3F3-79BC72CB2F71}"/>
+    <hyperlink ref="B6" r:id="rId83" xr:uid="{195279F9-EBFE-4437-9FB8-0BBFF3580365}"/>
+    <hyperlink ref="B12" r:id="rId84" xr:uid="{4FBEDC83-70C0-49F0-8235-3A3EB38A313B}"/>
+    <hyperlink ref="B13" r:id="rId85" xr:uid="{7114DE0A-D2B1-4167-A202-A636D2CD94E7}"/>
+    <hyperlink ref="B14" r:id="rId86" xr:uid="{0CE255C1-32AB-47C4-A4CC-30EEB4E0069F}"/>
+    <hyperlink ref="B15" r:id="rId87" xr:uid="{54836F6F-10D5-4D2D-BBA3-9D930D2A53F5}"/>
+    <hyperlink ref="B16" r:id="rId88" xr:uid="{8CA18949-2E98-4EA7-90C0-22D92C1AF01A}"/>
+    <hyperlink ref="B17" r:id="rId89" xr:uid="{7D3FE5EC-42BC-4F24-8C81-536BB585E10D}"/>
+    <hyperlink ref="B18" r:id="rId90" xr:uid="{939868F0-1934-476B-99CC-A2EEE9206BB4}"/>
+    <hyperlink ref="B19" r:id="rId91" xr:uid="{B93391F3-572A-46F1-A406-B5B4016D3BEC}"/>
+    <hyperlink ref="B20" r:id="rId92" xr:uid="{B52FBBDC-DACA-47F3-B833-04CE54B8D3D4}"/>
+    <hyperlink ref="B21" r:id="rId93" xr:uid="{1C8EB11E-EEB8-4187-95E5-719FC5918030}"/>
+    <hyperlink ref="B22" r:id="rId94" xr:uid="{DCC94920-B0C0-48F8-A23C-4E61FD99AA85}"/>
+    <hyperlink ref="B23" r:id="rId95" xr:uid="{980C8379-2947-42FD-9277-EC0B9415E26A}"/>
+    <hyperlink ref="B27" r:id="rId96" xr:uid="{A63DC6A0-DAA0-47B4-B86E-81BEF7722D70}"/>
+    <hyperlink ref="B28" r:id="rId97" xr:uid="{768AD13A-C993-4CE2-9E7A-0D1775A95D57}"/>
+    <hyperlink ref="B29" r:id="rId98" xr:uid="{151C6B22-69FC-4979-96F4-CCD927CA4CB0}"/>
+    <hyperlink ref="B30" r:id="rId99" xr:uid="{05E5506B-30A6-4174-BC91-41D4015993C7}"/>
+    <hyperlink ref="B31" r:id="rId100" xr:uid="{797EA4ED-0D39-45AE-A997-D194F3E6B4CC}"/>
+    <hyperlink ref="B32" r:id="rId101" xr:uid="{68A5811D-55F8-43D4-8C37-88AE27596814}"/>
+    <hyperlink ref="B33" r:id="rId102" xr:uid="{13E6ED39-1085-43F2-B562-580A1E5C9A68}"/>
+    <hyperlink ref="B34" r:id="rId103" xr:uid="{6FEEAB05-2858-4D56-B177-753CB54A3F26}"/>
+    <hyperlink ref="B35" r:id="rId104" xr:uid="{84695A3D-B6ED-4614-AA24-2EE1026C6A39}"/>
+    <hyperlink ref="B36" r:id="rId105" xr:uid="{D843727A-BEE5-4A68-82C5-AEB08659F485}"/>
+    <hyperlink ref="B37" r:id="rId106" xr:uid="{3F4F108E-6CB7-41B6-ABFC-91A197B55B86}"/>
+    <hyperlink ref="B38" r:id="rId107" xr:uid="{25A5B2B9-9171-43F8-8324-465107EF833A}"/>
+    <hyperlink ref="B39" r:id="rId108" xr:uid="{3608D9E5-8A75-4BE2-BADF-361FD3964112}"/>
+    <hyperlink ref="B40" r:id="rId109" xr:uid="{946191D8-EBA2-4E42-A903-2F65F9D442E8}"/>
+    <hyperlink ref="B41" r:id="rId110" xr:uid="{A07866FD-FDE3-464C-A17A-C0125D996D45}"/>
+    <hyperlink ref="B42" r:id="rId111" xr:uid="{AC919AB0-EE6A-4CC5-BCC5-B363E826E170}"/>
+    <hyperlink ref="B43" r:id="rId112" xr:uid="{2C80B518-3AC8-4D26-AD63-AAE4FC876ACF}"/>
+    <hyperlink ref="B24" r:id="rId113" xr:uid="{F25D957F-18D7-4EBE-ADC9-F24B4B2E4FB4}"/>
+    <hyperlink ref="B25" r:id="rId114" xr:uid="{4B08F1B1-4FCF-4181-9E94-0FD5E1D88CAB}"/>
+    <hyperlink ref="B4" r:id="rId115" xr:uid="{F364446A-6551-4E28-B9FD-EB52D867C3DA}"/>
+    <hyperlink ref="B3" r:id="rId116" display="https://archive.org/download/dli.ministry.16991/E14072_Memoirs_of_Baron_Bunsen_vol_I_djvu.txt " xr:uid="{1A0F21FD-2E30-47E5-BE1D-165F2416EBDB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId81"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId117"/>
 </worksheet>
 </file>
 
@@ -1194,17 +1533,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A444E4101166CB49B259A75BDE06F3BF" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8fffe44c5f6743ad9c8f54f3a4140bb9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6" xmlns:ns3="d6ffb985-a7ae-40c0-906d-05d0dcf51054" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ebb18812c57835850e1af3023911189" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A444E4101166CB49B259A75BDE06F3BF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c91372b7863c0478c61fa67c293378c4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6" xmlns:ns3="d6ffb985-a7ae-40c0-906d-05d0dcf51054" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a3a38847a6f132d9bcf9d24d77791a1" ns2:_="" ns3:_="">
     <xsd:import namespace="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6"/>
     <xsd:import namespace="d6ffb985-a7ae-40c0-906d-05d0dcf51054"/>
     <xsd:element name="properties">
@@ -1225,6 +1555,7 @@
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1287,6 +1618,11 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1419,38 +1755,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3809E15F-1619-45BE-A47F-8EFA477A2147}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3809E15F-1619-45BE-A47F-8EFA477A2147}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CEEFD53-950C-4833-817B-F8EB7FBC7DDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C74ED012-A405-4E19-B45B-715E1B33BE94}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB23CCD6-A20A-48B2-9136-03E8C25C1E2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6"/>
-    <ds:schemaRef ds:uri="d6ffb985-a7ae-40c0-906d-05d0dcf51054"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CEEFD53-950C-4833-817B-F8EB7FBC7DDC}"/>
 </file>
</xml_diff>